<commit_message>
list of Fall 30 Lohnartbeschreibungen + detection +-
</commit_message>
<xml_diff>
--- a/Dummymappe1.xlsx
+++ b/Dummymappe1.xlsx
@@ -1,21 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xml:space="preserve">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr codeName="ThisWorkbook"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Martina\Desktop\škola\informatika\git.projectinf\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView activeTab="0" autoFilterDateGrouping="true" firstSheet="0" minimized="false" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="600" visibility="visible"/>
+    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5688"/>
   </bookViews>
   <sheets>
-    <sheet name="Worksheet" sheetId="1" r:id="rId4"/>
+    <sheet name="Worksheet" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr calcId="999999" calcMode="auto" calcCompleted="1" fullCalcOnLoad="0" forceFullCalc="0"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="38">
   <si>
     <t>Firma</t>
   </si>
@@ -134,14 +138,9 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xml:space="preserve">
-  <numFmts count="0"/>
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
-      <b val="0"/>
-      <i val="0"/>
-      <strike val="0"/>
-      <u val="none"/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
@@ -152,28 +151,37 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="gray125">
-        <fgColor rgb="FFFFFFFF"/>
-        <bgColor rgb="FF000000"/>
-      </patternFill>
+      <patternFill patternType="gray125"/>
     </fill>
   </fills>
   <borders count="1">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normální" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotTableStyle1"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -463,19 +471,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xml:space="preserve" mc:Ignorable="x14ac">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="L5" sqref="L5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="12" max="12" width="18.44140625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:17">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -528,7 +536,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:17">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1002000</v>
       </c>
@@ -572,7 +580,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:17">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>1002000</v>
       </c>
@@ -619,7 +627,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:17">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>1002000</v>
       </c>
@@ -666,7 +674,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:17">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>1002000</v>
       </c>
@@ -707,7 +715,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="6" spans="1:17">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>1002000</v>
       </c>
@@ -748,7 +756,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:17">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>1002000</v>
       </c>
@@ -789,7 +797,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:17">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>1002000</v>
       </c>
@@ -830,7 +838,7 @@
         <v>9000</v>
       </c>
     </row>
-    <row r="9" spans="1:17">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>1002000</v>
       </c>
@@ -871,7 +879,7 @@
         <v>9000</v>
       </c>
     </row>
-    <row r="10" spans="1:17">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>1002000</v>
       </c>
@@ -912,7 +920,7 @@
         <v>9000</v>
       </c>
     </row>
-    <row r="11" spans="1:17">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>1002000</v>
       </c>
@@ -953,7 +961,7 @@
         <v>9000</v>
       </c>
     </row>
-    <row r="12" spans="1:17">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>1002000</v>
       </c>
@@ -994,7 +1002,7 @@
         <v>9000</v>
       </c>
     </row>
-    <row r="13" spans="1:17">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>1002000</v>
       </c>
@@ -1036,17 +1044,8 @@
       </c>
     </row>
   </sheetData>
-  <sheetProtection sheet="false" objects="false" scenarios="false" formatCells="false" formatColumns="false" formatRows="false" insertColumns="false" insertRows="false" insertHyperlinks="false" deleteColumns="false" deleteRows="false" selectLockedCells="false" sort="false" autoFilter="false" pivotTables="false" selectUnlockedCells="false"/>
-  <printOptions gridLines="false" gridLinesSet="true"/>
+  <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="1" orientation="default" scale="100" fitToHeight="1" fitToWidth="1"/>
-  <headerFooter differentOddEven="false" differentFirst="false" scaleWithDoc="true" alignWithMargins="true">
-    <oddHeader/>
-    <oddFooter/>
-    <evenHeader/>
-    <evenFooter/>
-    <firstHeader/>
-    <firstFooter/>
-  </headerFooter>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Finding column with names and Lohnarten
</commit_message>
<xml_diff>
--- a/Dummymappe1.xlsx
+++ b/Dummymappe1.xlsx
@@ -54,9 +54,6 @@
     <t>Lohnart</t>
   </si>
   <si>
-    <t>Lohnartbescreibung</t>
-  </si>
-  <si>
     <t>Zeit</t>
   </si>
   <si>
@@ -139,6 +136,9 @@
   </si>
   <si>
     <t>Pan yes</t>
+  </si>
+  <si>
+    <t>Lohnartbeschreibung</t>
   </si>
 </sst>
 </file>
@@ -480,8 +480,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B4" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="L1" sqref="L1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -524,22 +524,22 @@
         <v>10</v>
       </c>
       <c r="L1" t="s">
+        <v>39</v>
+      </c>
+      <c r="M1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>14</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>15</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.3">
@@ -550,7 +550,7 @@
         <v>44444</v>
       </c>
       <c r="C2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D2">
         <v>8</v>
@@ -577,13 +577,13 @@
         <v>610001</v>
       </c>
       <c r="L2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="M2">
         <v>39</v>
       </c>
       <c r="O2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.3">
@@ -594,7 +594,7 @@
         <v>44444</v>
       </c>
       <c r="C3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D3">
         <v>8</v>
@@ -621,7 +621,7 @@
         <v>702901</v>
       </c>
       <c r="L3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="M3">
         <v>2</v>
@@ -630,7 +630,7 @@
         <v>0</v>
       </c>
       <c r="O3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.3">
@@ -641,7 +641,7 @@
         <v>44444</v>
       </c>
       <c r="C4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D4">
         <v>8</v>
@@ -668,16 +668,16 @@
         <v>702901</v>
       </c>
       <c r="L4" t="s">
+        <v>19</v>
+      </c>
+      <c r="M4" t="s">
         <v>20</v>
       </c>
-      <c r="M4" t="s">
-        <v>21</v>
-      </c>
       <c r="N4">
         <v>0</v>
       </c>
       <c r="O4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.3">
@@ -688,7 +688,7 @@
         <v>44444</v>
       </c>
       <c r="C5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D5">
         <v>8</v>
@@ -715,10 +715,10 @@
         <v>703025</v>
       </c>
       <c r="L5" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q5" t="s">
         <v>22</v>
-      </c>
-      <c r="Q5" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.3">
@@ -729,7 +729,7 @@
         <v>44444</v>
       </c>
       <c r="C6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D6">
         <v>8</v>
@@ -756,7 +756,7 @@
         <v>751510</v>
       </c>
       <c r="L6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="Q6">
         <v>4</v>
@@ -770,7 +770,7 @@
         <v>44444</v>
       </c>
       <c r="C7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D7">
         <v>8</v>
@@ -797,7 +797,7 @@
         <v>789001</v>
       </c>
       <c r="L7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="P7">
         <v>4</v>
@@ -811,7 +811,7 @@
         <v>44444</v>
       </c>
       <c r="C8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D8">
         <v>8</v>
@@ -835,10 +835,10 @@
         <v>0</v>
       </c>
       <c r="K8" t="s">
+        <v>25</v>
+      </c>
+      <c r="L8" t="s">
         <v>26</v>
-      </c>
-      <c r="L8" t="s">
-        <v>27</v>
       </c>
       <c r="P8">
         <v>9000</v>
@@ -852,7 +852,7 @@
         <v>44444</v>
       </c>
       <c r="C9" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D9">
         <v>8</v>
@@ -876,10 +876,10 @@
         <v>0</v>
       </c>
       <c r="K9" t="s">
+        <v>27</v>
+      </c>
+      <c r="L9" t="s">
         <v>28</v>
-      </c>
-      <c r="L9" t="s">
-        <v>29</v>
       </c>
       <c r="Q9">
         <v>9000</v>
@@ -893,7 +893,7 @@
         <v>44444</v>
       </c>
       <c r="C10" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D10">
         <v>8</v>
@@ -917,10 +917,10 @@
         <v>0</v>
       </c>
       <c r="K10" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="L10" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="P10">
         <v>9000</v>
@@ -934,7 +934,7 @@
         <v>44444</v>
       </c>
       <c r="C11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D11">
         <v>8</v>
@@ -958,10 +958,10 @@
         <v>0</v>
       </c>
       <c r="K11" t="s">
+        <v>31</v>
+      </c>
+      <c r="L11" t="s">
         <v>32</v>
-      </c>
-      <c r="L11" t="s">
-        <v>33</v>
       </c>
       <c r="Q11">
         <v>9000</v>
@@ -975,7 +975,7 @@
         <v>44444</v>
       </c>
       <c r="C12" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D12">
         <v>8</v>
@@ -999,10 +999,10 @@
         <v>0</v>
       </c>
       <c r="K12" t="s">
+        <v>33</v>
+      </c>
+      <c r="L12" t="s">
         <v>34</v>
-      </c>
-      <c r="L12" t="s">
-        <v>35</v>
       </c>
       <c r="P12">
         <v>9000</v>
@@ -1016,7 +1016,7 @@
         <v>44444</v>
       </c>
       <c r="C13" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D13">
         <v>8</v>
@@ -1040,10 +1040,10 @@
         <v>0</v>
       </c>
       <c r="K13" t="s">
+        <v>35</v>
+      </c>
+      <c r="L13" t="s">
         <v>36</v>
-      </c>
-      <c r="L13" t="s">
-        <v>37</v>
       </c>
       <c r="M13">
         <v>25</v>
@@ -1051,34 +1051,34 @@
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.3">
       <c r="C14" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="L14" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.3">
       <c r="C15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="L15" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.3">
       <c r="C16" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="L16" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="17" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C17" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="L17" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
number of columns changed to letter
</commit_message>
<xml_diff>
--- a/Dummymappe1.xlsx
+++ b/Dummymappe1.xlsx
@@ -480,8 +480,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="L1" sqref="L1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
List with month count!
</commit_message>
<xml_diff>
--- a/Dummymappe1.xlsx
+++ b/Dummymappe1.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="40">
   <si>
     <t>Firma</t>
   </si>
@@ -478,10 +478,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q17"/>
+  <dimension ref="A1:Q19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="D18" sqref="D18:D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1053,6 +1053,9 @@
       <c r="C14" t="s">
         <v>37</v>
       </c>
+      <c r="D14">
+        <v>8</v>
+      </c>
       <c r="L14" t="s">
         <v>17</v>
       </c>
@@ -1061,6 +1064,9 @@
       <c r="C15" t="s">
         <v>37</v>
       </c>
+      <c r="D15">
+        <v>9</v>
+      </c>
       <c r="L15" t="s">
         <v>30</v>
       </c>
@@ -1069,6 +1075,9 @@
       <c r="C16" t="s">
         <v>38</v>
       </c>
+      <c r="D16">
+        <v>9</v>
+      </c>
       <c r="L16" t="s">
         <v>26</v>
       </c>
@@ -1077,8 +1086,27 @@
       <c r="C17" t="s">
         <v>38</v>
       </c>
+      <c r="D17">
+        <v>9</v>
+      </c>
       <c r="L17" t="s">
         <v>30</v>
+      </c>
+    </row>
+    <row r="18" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C18" t="s">
+        <v>38</v>
+      </c>
+      <c r="D18">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="19" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C19" t="s">
+        <v>38</v>
+      </c>
+      <c r="D19">
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
all names and months in final excel alligned
</commit_message>
<xml_diff>
--- a/Dummymappe1.xlsx
+++ b/Dummymappe1.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="44">
   <si>
     <t>Firma</t>
   </si>
@@ -139,6 +139,18 @@
   </si>
   <si>
     <t>Lohnartbeschreibung</t>
+  </si>
+  <si>
+    <t>Pan hes</t>
+  </si>
+  <si>
+    <t>Pan kes</t>
+  </si>
+  <si>
+    <t>pan qes</t>
+  </si>
+  <si>
+    <t>pan bes</t>
   </si>
 </sst>
 </file>
@@ -478,10 +490,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q19"/>
+  <dimension ref="A1:Q28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18:D19"/>
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="L25" sqref="L25:L28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1100,6 +1112,9 @@
       <c r="D18">
         <v>8</v>
       </c>
+      <c r="L18" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="19" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C19" t="s">
@@ -1107,6 +1122,108 @@
       </c>
       <c r="D19">
         <v>8</v>
+      </c>
+      <c r="L19" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="20" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C20" t="s">
+        <v>40</v>
+      </c>
+      <c r="D20">
+        <v>4</v>
+      </c>
+      <c r="L20" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="21" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C21" t="s">
+        <v>40</v>
+      </c>
+      <c r="D21">
+        <v>3</v>
+      </c>
+      <c r="L21" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="22" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C22" t="s">
+        <v>40</v>
+      </c>
+      <c r="D22">
+        <v>3</v>
+      </c>
+      <c r="L22" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="23" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C23" t="s">
+        <v>41</v>
+      </c>
+      <c r="D23">
+        <v>9</v>
+      </c>
+      <c r="L23" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="24" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C24" t="s">
+        <v>41</v>
+      </c>
+      <c r="D24">
+        <v>4</v>
+      </c>
+      <c r="L24" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="25" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C25" t="s">
+        <v>42</v>
+      </c>
+      <c r="D25">
+        <v>6</v>
+      </c>
+      <c r="L25" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="26" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C26" t="s">
+        <v>42</v>
+      </c>
+      <c r="D26">
+        <v>6</v>
+      </c>
+      <c r="L26" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="27" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C27" t="s">
+        <v>43</v>
+      </c>
+      <c r="D27">
+        <v>8</v>
+      </c>
+      <c r="L27" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="28" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C28" t="s">
+        <v>43</v>
+      </c>
+      <c r="D28">
+        <v>8</v>
+      </c>
+      <c r="L28" t="s">
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
naming letters of columns
</commit_message>
<xml_diff>
--- a/Dummymappe1.xlsx
+++ b/Dummymappe1.xlsx
@@ -157,11 +157,18 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
     </font>
   </fonts>
   <fills count="2">
@@ -184,8 +191,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normální" xfId="0" builtinId="0"/>
@@ -490,10 +498,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q28"/>
+  <dimension ref="AA1:AQ28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="L25" sqref="L25:L28"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="AA1" sqref="AA1:AQ28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -501,728 +509,728 @@
     <col min="12" max="12" width="18.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
+    <row r="1" spans="27:43" x14ac:dyDescent="0.3">
+      <c r="AA1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AB1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="AC1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="AD1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="AE1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="AF1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="AG1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="AH1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" t="s">
+      <c r="AI1" t="s">
+        <v>8</v>
+      </c>
+      <c r="AJ1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s">
+      <c r="AK1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" t="s">
+      <c r="AL1" t="s">
         <v>39</v>
       </c>
-      <c r="M1" t="s">
+      <c r="AM1" t="s">
         <v>11</v>
       </c>
-      <c r="N1" t="s">
+      <c r="AN1" t="s">
         <v>12</v>
       </c>
-      <c r="O1" t="s">
+      <c r="AO1" t="s">
         <v>13</v>
       </c>
-      <c r="P1" t="s">
+      <c r="AP1" t="s">
         <v>14</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="AQ1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A2">
+    <row r="2" spans="27:43" x14ac:dyDescent="0.3">
+      <c r="AA2">
         <v>1002000</v>
       </c>
-      <c r="B2">
+      <c r="AB2">
         <v>44444</v>
       </c>
-      <c r="C2" t="s">
+      <c r="AC2" t="s">
         <v>16</v>
       </c>
-      <c r="D2">
-        <v>8</v>
-      </c>
-      <c r="E2">
+      <c r="AD2">
+        <v>8</v>
+      </c>
+      <c r="AE2">
         <v>2024</v>
       </c>
-      <c r="F2">
+      <c r="AF2">
         <v>5468</v>
       </c>
-      <c r="G2">
-        <v>30</v>
-      </c>
-      <c r="H2">
+      <c r="AG2">
+        <v>30</v>
+      </c>
+      <c r="AH2">
         <v>31</v>
       </c>
-      <c r="I2">
+      <c r="AI2">
         <v>1</v>
       </c>
-      <c r="J2">
-        <v>0</v>
-      </c>
-      <c r="K2">
+      <c r="AJ2">
+        <v>0</v>
+      </c>
+      <c r="AK2">
         <v>610001</v>
       </c>
-      <c r="L2" t="s">
+      <c r="AL2" t="s">
         <v>17</v>
       </c>
-      <c r="M2">
+      <c r="AM2">
         <v>39</v>
       </c>
-      <c r="O2" t="s">
+      <c r="AO2" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A3">
+    <row r="3" spans="27:43" x14ac:dyDescent="0.3">
+      <c r="AA3">
         <v>1002000</v>
       </c>
-      <c r="B3">
+      <c r="AB3">
         <v>44444</v>
       </c>
-      <c r="C3" t="s">
+      <c r="AC3" t="s">
         <v>16</v>
       </c>
-      <c r="D3">
-        <v>8</v>
-      </c>
-      <c r="E3">
+      <c r="AD3">
+        <v>8</v>
+      </c>
+      <c r="AE3">
         <v>2024</v>
       </c>
-      <c r="F3">
+      <c r="AF3">
         <v>5468</v>
       </c>
-      <c r="G3">
-        <v>30</v>
-      </c>
-      <c r="H3">
+      <c r="AG3">
+        <v>30</v>
+      </c>
+      <c r="AH3">
         <v>31</v>
       </c>
-      <c r="I3">
+      <c r="AI3">
         <v>1</v>
       </c>
-      <c r="J3">
-        <v>0</v>
-      </c>
-      <c r="K3">
+      <c r="AJ3">
+        <v>0</v>
+      </c>
+      <c r="AK3">
         <v>702901</v>
       </c>
-      <c r="L3" t="s">
+      <c r="AL3" t="s">
         <v>19</v>
       </c>
-      <c r="M3">
+      <c r="AM3">
         <v>2</v>
       </c>
-      <c r="N3">
-        <v>0</v>
-      </c>
-      <c r="O3" t="s">
+      <c r="AN3">
+        <v>0</v>
+      </c>
+      <c r="AO3" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A4">
+    <row r="4" spans="27:43" x14ac:dyDescent="0.3">
+      <c r="AA4">
         <v>1002000</v>
       </c>
-      <c r="B4">
+      <c r="AB4">
         <v>44444</v>
       </c>
-      <c r="C4" t="s">
+      <c r="AC4" t="s">
         <v>16</v>
       </c>
-      <c r="D4">
-        <v>8</v>
-      </c>
-      <c r="E4">
+      <c r="AD4">
+        <v>8</v>
+      </c>
+      <c r="AE4">
         <v>2024</v>
       </c>
-      <c r="F4">
+      <c r="AF4">
         <v>5468</v>
       </c>
-      <c r="G4">
-        <v>30</v>
-      </c>
-      <c r="H4">
+      <c r="AG4">
+        <v>30</v>
+      </c>
+      <c r="AH4">
         <v>31</v>
       </c>
-      <c r="I4">
+      <c r="AI4">
         <v>1</v>
       </c>
-      <c r="J4">
-        <v>0</v>
-      </c>
-      <c r="K4">
+      <c r="AJ4">
+        <v>0</v>
+      </c>
+      <c r="AK4">
         <v>702901</v>
       </c>
-      <c r="L4" t="s">
+      <c r="AL4" t="s">
         <v>19</v>
       </c>
-      <c r="M4" t="s">
+      <c r="AM4" t="s">
         <v>20</v>
       </c>
-      <c r="N4">
-        <v>0</v>
-      </c>
-      <c r="O4" t="s">
+      <c r="AN4">
+        <v>0</v>
+      </c>
+      <c r="AO4" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A5">
+    <row r="5" spans="27:43" x14ac:dyDescent="0.3">
+      <c r="AA5">
         <v>1002000</v>
       </c>
-      <c r="B5">
+      <c r="AB5">
         <v>44444</v>
       </c>
-      <c r="C5" t="s">
+      <c r="AC5" t="s">
         <v>16</v>
       </c>
-      <c r="D5">
-        <v>8</v>
-      </c>
-      <c r="E5">
+      <c r="AD5">
+        <v>8</v>
+      </c>
+      <c r="AE5">
         <v>2024</v>
       </c>
-      <c r="F5">
+      <c r="AF5">
         <v>5468</v>
       </c>
-      <c r="G5">
-        <v>30</v>
-      </c>
-      <c r="H5">
+      <c r="AG5">
+        <v>30</v>
+      </c>
+      <c r="AH5">
         <v>31</v>
       </c>
-      <c r="I5">
+      <c r="AI5">
         <v>1</v>
       </c>
-      <c r="J5">
-        <v>0</v>
-      </c>
-      <c r="K5">
+      <c r="AJ5">
+        <v>0</v>
+      </c>
+      <c r="AK5">
         <v>703025</v>
       </c>
-      <c r="L5" t="s">
+      <c r="AL5" t="s">
         <v>21</v>
       </c>
-      <c r="Q5" t="s">
+      <c r="AQ5" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A6">
+    <row r="6" spans="27:43" x14ac:dyDescent="0.3">
+      <c r="AA6">
         <v>1002000</v>
       </c>
-      <c r="B6">
+      <c r="AB6">
         <v>44444</v>
       </c>
-      <c r="C6" t="s">
+      <c r="AC6" t="s">
         <v>16</v>
       </c>
-      <c r="D6">
-        <v>8</v>
-      </c>
-      <c r="E6">
+      <c r="AD6">
+        <v>8</v>
+      </c>
+      <c r="AE6">
         <v>2024</v>
       </c>
-      <c r="F6">
+      <c r="AF6">
         <v>5468</v>
       </c>
-      <c r="G6">
-        <v>30</v>
-      </c>
-      <c r="H6">
+      <c r="AG6">
+        <v>30</v>
+      </c>
+      <c r="AH6">
         <v>31</v>
       </c>
-      <c r="I6">
+      <c r="AI6">
         <v>1</v>
       </c>
-      <c r="J6">
-        <v>0</v>
-      </c>
-      <c r="K6">
+      <c r="AJ6">
+        <v>0</v>
+      </c>
+      <c r="AK6">
         <v>751510</v>
       </c>
-      <c r="L6" t="s">
+      <c r="AL6" t="s">
         <v>23</v>
       </c>
-      <c r="Q6">
+      <c r="AQ6">
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A7">
+    <row r="7" spans="27:43" x14ac:dyDescent="0.3">
+      <c r="AA7">
         <v>1002000</v>
       </c>
-      <c r="B7">
+      <c r="AB7">
         <v>44444</v>
       </c>
-      <c r="C7" t="s">
+      <c r="AC7" t="s">
         <v>16</v>
       </c>
-      <c r="D7">
-        <v>8</v>
-      </c>
-      <c r="E7">
+      <c r="AD7">
+        <v>8</v>
+      </c>
+      <c r="AE7">
         <v>2024</v>
       </c>
-      <c r="F7">
+      <c r="AF7">
         <v>5468</v>
       </c>
-      <c r="G7">
-        <v>30</v>
-      </c>
-      <c r="H7">
+      <c r="AG7">
+        <v>30</v>
+      </c>
+      <c r="AH7">
         <v>31</v>
       </c>
-      <c r="I7">
+      <c r="AI7">
         <v>1</v>
       </c>
-      <c r="J7">
-        <v>0</v>
-      </c>
-      <c r="K7">
+      <c r="AJ7">
+        <v>0</v>
+      </c>
+      <c r="AK7">
         <v>789001</v>
       </c>
-      <c r="L7" t="s">
+      <c r="AL7" t="s">
         <v>24</v>
       </c>
-      <c r="P7">
+      <c r="AP7">
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A8">
+    <row r="8" spans="27:43" x14ac:dyDescent="0.3">
+      <c r="AA8">
         <v>1002000</v>
       </c>
-      <c r="B8">
+      <c r="AB8">
         <v>44444</v>
       </c>
-      <c r="C8" t="s">
+      <c r="AC8" t="s">
         <v>16</v>
       </c>
-      <c r="D8">
-        <v>8</v>
-      </c>
-      <c r="E8">
+      <c r="AD8">
+        <v>8</v>
+      </c>
+      <c r="AE8">
         <v>2024</v>
       </c>
-      <c r="F8">
+      <c r="AF8">
         <v>5468</v>
       </c>
-      <c r="G8">
-        <v>30</v>
-      </c>
-      <c r="H8">
+      <c r="AG8">
+        <v>30</v>
+      </c>
+      <c r="AH8">
         <v>31</v>
       </c>
-      <c r="I8">
+      <c r="AI8">
         <v>1</v>
       </c>
-      <c r="J8">
-        <v>0</v>
-      </c>
-      <c r="K8" t="s">
+      <c r="AJ8">
+        <v>0</v>
+      </c>
+      <c r="AK8" t="s">
         <v>25</v>
       </c>
-      <c r="L8" t="s">
+      <c r="AL8" t="s">
         <v>26</v>
       </c>
-      <c r="P8">
+      <c r="AP8">
         <v>9000</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A9">
+    <row r="9" spans="27:43" x14ac:dyDescent="0.3">
+      <c r="AA9">
         <v>1002000</v>
       </c>
-      <c r="B9">
+      <c r="AB9">
         <v>44444</v>
       </c>
-      <c r="C9" t="s">
+      <c r="AC9" t="s">
         <v>16</v>
       </c>
-      <c r="D9">
-        <v>8</v>
-      </c>
-      <c r="E9">
+      <c r="AD9">
+        <v>8</v>
+      </c>
+      <c r="AE9">
         <v>2024</v>
       </c>
-      <c r="F9">
+      <c r="AF9">
         <v>5468</v>
       </c>
-      <c r="G9">
-        <v>30</v>
-      </c>
-      <c r="H9">
+      <c r="AG9">
+        <v>30</v>
+      </c>
+      <c r="AH9">
         <v>31</v>
       </c>
-      <c r="I9">
+      <c r="AI9">
         <v>1</v>
       </c>
-      <c r="J9">
-        <v>0</v>
-      </c>
-      <c r="K9" t="s">
+      <c r="AJ9">
+        <v>0</v>
+      </c>
+      <c r="AK9" t="s">
         <v>27</v>
       </c>
-      <c r="L9" t="s">
+      <c r="AL9" t="s">
         <v>28</v>
       </c>
-      <c r="Q9">
+      <c r="AQ9">
         <v>9000</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A10">
+    <row r="10" spans="27:43" x14ac:dyDescent="0.3">
+      <c r="AA10">
         <v>1002000</v>
       </c>
-      <c r="B10">
+      <c r="AB10">
         <v>44444</v>
       </c>
-      <c r="C10" t="s">
+      <c r="AC10" t="s">
         <v>16</v>
       </c>
-      <c r="D10">
-        <v>8</v>
-      </c>
-      <c r="E10">
+      <c r="AD10">
+        <v>8</v>
+      </c>
+      <c r="AE10">
         <v>2024</v>
       </c>
-      <c r="F10">
+      <c r="AF10">
         <v>5468</v>
       </c>
-      <c r="G10">
-        <v>30</v>
-      </c>
-      <c r="H10">
+      <c r="AG10">
+        <v>30</v>
+      </c>
+      <c r="AH10">
         <v>31</v>
       </c>
-      <c r="I10">
+      <c r="AI10">
         <v>1</v>
       </c>
-      <c r="J10">
-        <v>0</v>
-      </c>
-      <c r="K10" t="s">
+      <c r="AJ10">
+        <v>0</v>
+      </c>
+      <c r="AK10" t="s">
         <v>29</v>
       </c>
-      <c r="L10" t="s">
-        <v>30</v>
-      </c>
-      <c r="P10">
+      <c r="AL10" t="s">
+        <v>30</v>
+      </c>
+      <c r="AP10">
         <v>9000</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A11">
+    <row r="11" spans="27:43" x14ac:dyDescent="0.3">
+      <c r="AA11">
         <v>1002000</v>
       </c>
-      <c r="B11">
+      <c r="AB11">
         <v>44444</v>
       </c>
-      <c r="C11" t="s">
+      <c r="AC11" t="s">
         <v>16</v>
       </c>
-      <c r="D11">
-        <v>8</v>
-      </c>
-      <c r="E11">
+      <c r="AD11">
+        <v>8</v>
+      </c>
+      <c r="AE11">
         <v>2024</v>
       </c>
-      <c r="F11">
+      <c r="AF11">
         <v>5468</v>
       </c>
-      <c r="G11">
-        <v>30</v>
-      </c>
-      <c r="H11">
+      <c r="AG11">
+        <v>30</v>
+      </c>
+      <c r="AH11">
         <v>31</v>
       </c>
-      <c r="I11">
+      <c r="AI11">
         <v>1</v>
       </c>
-      <c r="J11">
-        <v>0</v>
-      </c>
-      <c r="K11" t="s">
+      <c r="AJ11">
+        <v>0</v>
+      </c>
+      <c r="AK11" t="s">
         <v>31</v>
       </c>
-      <c r="L11" t="s">
+      <c r="AL11" t="s">
         <v>32</v>
       </c>
-      <c r="Q11">
+      <c r="AQ11">
         <v>9000</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A12">
+    <row r="12" spans="27:43" x14ac:dyDescent="0.3">
+      <c r="AA12">
         <v>1002000</v>
       </c>
-      <c r="B12">
+      <c r="AB12">
         <v>44444</v>
       </c>
-      <c r="C12" t="s">
+      <c r="AC12" t="s">
         <v>16</v>
       </c>
-      <c r="D12">
-        <v>8</v>
-      </c>
-      <c r="E12">
+      <c r="AD12">
+        <v>8</v>
+      </c>
+      <c r="AE12">
         <v>2024</v>
       </c>
-      <c r="F12">
+      <c r="AF12">
         <v>5468</v>
       </c>
-      <c r="G12">
-        <v>30</v>
-      </c>
-      <c r="H12">
+      <c r="AG12">
+        <v>30</v>
+      </c>
+      <c r="AH12">
         <v>31</v>
       </c>
-      <c r="I12">
+      <c r="AI12">
         <v>1</v>
       </c>
-      <c r="J12">
-        <v>0</v>
-      </c>
-      <c r="K12" t="s">
+      <c r="AJ12">
+        <v>0</v>
+      </c>
+      <c r="AK12" t="s">
         <v>33</v>
       </c>
-      <c r="L12" t="s">
+      <c r="AL12" t="s">
         <v>34</v>
       </c>
-      <c r="P12">
+      <c r="AP12">
         <v>9000</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A13">
+    <row r="13" spans="27:43" x14ac:dyDescent="0.3">
+      <c r="AA13">
         <v>1002000</v>
       </c>
-      <c r="B13">
+      <c r="AB13">
         <v>44444</v>
       </c>
-      <c r="C13" t="s">
+      <c r="AC13" t="s">
         <v>16</v>
       </c>
-      <c r="D13">
-        <v>8</v>
-      </c>
-      <c r="E13">
+      <c r="AD13">
+        <v>8</v>
+      </c>
+      <c r="AE13">
         <v>2024</v>
       </c>
-      <c r="F13">
+      <c r="AF13">
         <v>5468</v>
       </c>
-      <c r="G13">
-        <v>30</v>
-      </c>
-      <c r="H13">
+      <c r="AG13">
+        <v>30</v>
+      </c>
+      <c r="AH13">
         <v>31</v>
       </c>
-      <c r="I13">
+      <c r="AI13">
         <v>1</v>
       </c>
-      <c r="J13">
-        <v>0</v>
-      </c>
-      <c r="K13" t="s">
+      <c r="AJ13">
+        <v>0</v>
+      </c>
+      <c r="AK13" t="s">
         <v>35</v>
       </c>
-      <c r="L13" t="s">
+      <c r="AL13" t="s">
         <v>36</v>
       </c>
-      <c r="M13">
+      <c r="AM13">
         <v>25</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="C14" t="s">
+    <row r="14" spans="27:43" x14ac:dyDescent="0.3">
+      <c r="AC14" t="s">
         <v>37</v>
       </c>
-      <c r="D14">
-        <v>8</v>
-      </c>
-      <c r="L14" t="s">
+      <c r="AD14">
+        <v>8</v>
+      </c>
+      <c r="AL14" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="C15" t="s">
+    <row r="15" spans="27:43" x14ac:dyDescent="0.3">
+      <c r="AC15" t="s">
         <v>37</v>
       </c>
-      <c r="D15">
+      <c r="AD15">
         <v>9</v>
       </c>
-      <c r="L15" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="C16" t="s">
+      <c r="AL15" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="16" spans="27:43" x14ac:dyDescent="0.3">
+      <c r="AC16" t="s">
         <v>38</v>
       </c>
-      <c r="D16">
+      <c r="AD16">
         <v>9</v>
       </c>
-      <c r="L16" t="s">
+      <c r="AL16" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="17" spans="3:12" x14ac:dyDescent="0.3">
-      <c r="C17" t="s">
+    <row r="17" spans="29:38" x14ac:dyDescent="0.3">
+      <c r="AC17" t="s">
         <v>38</v>
       </c>
-      <c r="D17">
+      <c r="AD17">
         <v>9</v>
       </c>
-      <c r="L17" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="18" spans="3:12" x14ac:dyDescent="0.3">
-      <c r="C18" t="s">
+      <c r="AL17" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="18" spans="29:38" x14ac:dyDescent="0.3">
+      <c r="AC18" t="s">
         <v>38</v>
       </c>
-      <c r="D18">
-        <v>8</v>
-      </c>
-      <c r="L18" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="19" spans="3:12" x14ac:dyDescent="0.3">
-      <c r="C19" t="s">
+      <c r="AD18">
+        <v>8</v>
+      </c>
+      <c r="AL18" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="19" spans="29:38" x14ac:dyDescent="0.3">
+      <c r="AC19" t="s">
         <v>38</v>
       </c>
-      <c r="D19">
-        <v>8</v>
-      </c>
-      <c r="L19" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="20" spans="3:12" x14ac:dyDescent="0.3">
-      <c r="C20" t="s">
+      <c r="AD19">
+        <v>8</v>
+      </c>
+      <c r="AL19" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="20" spans="29:38" x14ac:dyDescent="0.3">
+      <c r="AC20" t="s">
         <v>40</v>
       </c>
-      <c r="D20">
+      <c r="AD20">
         <v>4</v>
       </c>
-      <c r="L20" t="s">
+      <c r="AL20" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="21" spans="3:12" x14ac:dyDescent="0.3">
-      <c r="C21" t="s">
+    <row r="21" spans="29:38" x14ac:dyDescent="0.3">
+      <c r="AC21" t="s">
         <v>40</v>
       </c>
-      <c r="D21">
+      <c r="AD21">
         <v>3</v>
       </c>
-      <c r="L21" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="22" spans="3:12" x14ac:dyDescent="0.3">
-      <c r="C22" t="s">
+      <c r="AL21" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="22" spans="29:38" x14ac:dyDescent="0.3">
+      <c r="AC22" t="s">
         <v>40</v>
       </c>
-      <c r="D22">
+      <c r="AD22">
         <v>3</v>
       </c>
-      <c r="L22" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="23" spans="3:12" x14ac:dyDescent="0.3">
-      <c r="C23" t="s">
+      <c r="AL22" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="23" spans="29:38" x14ac:dyDescent="0.3">
+      <c r="AC23" t="s">
         <v>41</v>
       </c>
-      <c r="D23">
+      <c r="AD23">
         <v>9</v>
       </c>
-      <c r="L23" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="24" spans="3:12" x14ac:dyDescent="0.3">
-      <c r="C24" t="s">
+      <c r="AL23" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="24" spans="29:38" x14ac:dyDescent="0.3">
+      <c r="AC24" t="s">
         <v>41</v>
       </c>
-      <c r="D24">
+      <c r="AD24">
         <v>4</v>
       </c>
-      <c r="L24" t="s">
+      <c r="AL24" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="25" spans="3:12" x14ac:dyDescent="0.3">
-      <c r="C25" t="s">
+    <row r="25" spans="29:38" x14ac:dyDescent="0.3">
+      <c r="AC25" t="s">
         <v>42</v>
       </c>
-      <c r="D25">
+      <c r="AD25">
         <v>6</v>
       </c>
-      <c r="L25" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="26" spans="3:12" x14ac:dyDescent="0.3">
-      <c r="C26" t="s">
+      <c r="AL25" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="26" spans="29:38" x14ac:dyDescent="0.3">
+      <c r="AC26" t="s">
         <v>42</v>
       </c>
-      <c r="D26">
+      <c r="AD26">
         <v>6</v>
       </c>
-      <c r="L26" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="27" spans="3:12" x14ac:dyDescent="0.3">
-      <c r="C27" t="s">
+      <c r="AL26" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="27" spans="29:38" x14ac:dyDescent="0.3">
+      <c r="AC27" t="s">
         <v>43</v>
       </c>
-      <c r="D27">
-        <v>8</v>
-      </c>
-      <c r="L27" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="28" spans="3:12" x14ac:dyDescent="0.3">
-      <c r="C28" t="s">
+      <c r="AD27">
+        <v>8</v>
+      </c>
+      <c r="AL27" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="28" spans="29:38" x14ac:dyDescent="0.3">
+      <c r="AC28" t="s">
         <v>43</v>
       </c>
-      <c r="D28">
-        <v>8</v>
-      </c>
-      <c r="L28" t="s">
+      <c r="AD28">
+        <v>8</v>
+      </c>
+      <c r="AL28" t="s">
         <v>30</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Gesamtergebnis at the end of final report
</commit_message>
<xml_diff>
--- a/Dummymappe1.xlsx
+++ b/Dummymappe1.xlsx
@@ -500,8 +500,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="AA1:AQ28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="AA1" sqref="AA1:AQ28"/>
+    <sheetView tabSelected="1" topLeftCell="M1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="AC32" sqref="AC32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1070,6 +1070,12 @@
       </c>
     </row>
     <row r="14" spans="27:43" x14ac:dyDescent="0.3">
+      <c r="AA14">
+        <v>1002000</v>
+      </c>
+      <c r="AB14">
+        <v>555555</v>
+      </c>
       <c r="AC14" t="s">
         <v>37</v>
       </c>
@@ -1081,6 +1087,12 @@
       </c>
     </row>
     <row r="15" spans="27:43" x14ac:dyDescent="0.3">
+      <c r="AA15">
+        <v>1002000</v>
+      </c>
+      <c r="AB15">
+        <v>555555</v>
+      </c>
       <c r="AC15" t="s">
         <v>37</v>
       </c>
@@ -1092,6 +1104,12 @@
       </c>
     </row>
     <row r="16" spans="27:43" x14ac:dyDescent="0.3">
+      <c r="AA16">
+        <v>1002000</v>
+      </c>
+      <c r="AB16">
+        <v>6666</v>
+      </c>
       <c r="AC16" t="s">
         <v>38</v>
       </c>
@@ -1102,7 +1120,13 @@
         <v>26</v>
       </c>
     </row>
-    <row r="17" spans="29:38" x14ac:dyDescent="0.3">
+    <row r="17" spans="27:38" x14ac:dyDescent="0.3">
+      <c r="AA17">
+        <v>1002000</v>
+      </c>
+      <c r="AB17">
+        <v>6666</v>
+      </c>
       <c r="AC17" t="s">
         <v>38</v>
       </c>
@@ -1113,7 +1137,13 @@
         <v>30</v>
       </c>
     </row>
-    <row r="18" spans="29:38" x14ac:dyDescent="0.3">
+    <row r="18" spans="27:38" x14ac:dyDescent="0.3">
+      <c r="AA18">
+        <v>1002000</v>
+      </c>
+      <c r="AB18">
+        <v>6666</v>
+      </c>
       <c r="AC18" t="s">
         <v>38</v>
       </c>
@@ -1124,7 +1154,13 @@
         <v>30</v>
       </c>
     </row>
-    <row r="19" spans="29:38" x14ac:dyDescent="0.3">
+    <row r="19" spans="27:38" x14ac:dyDescent="0.3">
+      <c r="AA19">
+        <v>1002000</v>
+      </c>
+      <c r="AB19">
+        <v>6666</v>
+      </c>
       <c r="AC19" t="s">
         <v>38</v>
       </c>
@@ -1135,7 +1171,13 @@
         <v>30</v>
       </c>
     </row>
-    <row r="20" spans="29:38" x14ac:dyDescent="0.3">
+    <row r="20" spans="27:38" x14ac:dyDescent="0.3">
+      <c r="AA20">
+        <v>1002000</v>
+      </c>
+      <c r="AB20">
+        <v>777</v>
+      </c>
       <c r="AC20" t="s">
         <v>40</v>
       </c>
@@ -1146,7 +1188,13 @@
         <v>17</v>
       </c>
     </row>
-    <row r="21" spans="29:38" x14ac:dyDescent="0.3">
+    <row r="21" spans="27:38" x14ac:dyDescent="0.3">
+      <c r="AA21">
+        <v>1003000</v>
+      </c>
+      <c r="AB21">
+        <v>777</v>
+      </c>
       <c r="AC21" t="s">
         <v>40</v>
       </c>
@@ -1157,7 +1205,13 @@
         <v>30</v>
       </c>
     </row>
-    <row r="22" spans="29:38" x14ac:dyDescent="0.3">
+    <row r="22" spans="27:38" x14ac:dyDescent="0.3">
+      <c r="AA22">
+        <v>1003000</v>
+      </c>
+      <c r="AB22">
+        <v>777</v>
+      </c>
       <c r="AC22" t="s">
         <v>40</v>
       </c>
@@ -1168,7 +1222,13 @@
         <v>30</v>
       </c>
     </row>
-    <row r="23" spans="29:38" x14ac:dyDescent="0.3">
+    <row r="23" spans="27:38" x14ac:dyDescent="0.3">
+      <c r="AA23">
+        <v>1003000</v>
+      </c>
+      <c r="AB23">
+        <v>222</v>
+      </c>
       <c r="AC23" t="s">
         <v>41</v>
       </c>
@@ -1179,7 +1239,13 @@
         <v>30</v>
       </c>
     </row>
-    <row r="24" spans="29:38" x14ac:dyDescent="0.3">
+    <row r="24" spans="27:38" x14ac:dyDescent="0.3">
+      <c r="AA24">
+        <v>1003000</v>
+      </c>
+      <c r="AB24">
+        <v>222</v>
+      </c>
       <c r="AC24" t="s">
         <v>41</v>
       </c>
@@ -1190,7 +1256,13 @@
         <v>17</v>
       </c>
     </row>
-    <row r="25" spans="29:38" x14ac:dyDescent="0.3">
+    <row r="25" spans="27:38" x14ac:dyDescent="0.3">
+      <c r="AA25">
+        <v>1003000</v>
+      </c>
+      <c r="AB25">
+        <v>33</v>
+      </c>
       <c r="AC25" t="s">
         <v>42</v>
       </c>
@@ -1201,7 +1273,13 @@
         <v>30</v>
       </c>
     </row>
-    <row r="26" spans="29:38" x14ac:dyDescent="0.3">
+    <row r="26" spans="27:38" x14ac:dyDescent="0.3">
+      <c r="AA26">
+        <v>1003000</v>
+      </c>
+      <c r="AB26">
+        <v>33</v>
+      </c>
       <c r="AC26" t="s">
         <v>42</v>
       </c>
@@ -1212,7 +1290,13 @@
         <v>30</v>
       </c>
     </row>
-    <row r="27" spans="29:38" x14ac:dyDescent="0.3">
+    <row r="27" spans="27:38" x14ac:dyDescent="0.3">
+      <c r="AA27">
+        <v>1003000</v>
+      </c>
+      <c r="AB27">
+        <v>18</v>
+      </c>
       <c r="AC27" t="s">
         <v>43</v>
       </c>
@@ -1223,7 +1307,13 @@
         <v>30</v>
       </c>
     </row>
-    <row r="28" spans="29:38" x14ac:dyDescent="0.3">
+    <row r="28" spans="27:38" x14ac:dyDescent="0.3">
+      <c r="AA28">
+        <v>1003000</v>
+      </c>
+      <c r="AB28">
+        <v>18</v>
+      </c>
       <c r="AC28" t="s">
         <v>43</v>
       </c>

</xml_diff>

<commit_message>
Here we go again... - just Fall30 to go
</commit_message>
<xml_diff>
--- a/Dummymappe1.xlsx
+++ b/Dummymappe1.xlsx
@@ -498,10 +498,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="AA1:AQ28"/>
+  <dimension ref="A1:Q28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="AC32" sqref="AC32"/>
+    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection sqref="A1:Q28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -509,818 +509,818 @@
     <col min="12" max="12" width="18.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="27:43" x14ac:dyDescent="0.3">
-      <c r="AA1" t="s">
-        <v>0</v>
-      </c>
-      <c r="AB1" t="s">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="AC1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="AD1" t="s">
+      <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="AE1" t="s">
+      <c r="E1" t="s">
         <v>4</v>
       </c>
-      <c r="AF1" t="s">
+      <c r="F1" t="s">
         <v>5</v>
       </c>
-      <c r="AG1" t="s">
+      <c r="G1" t="s">
         <v>6</v>
       </c>
-      <c r="AH1" t="s">
+      <c r="H1" t="s">
         <v>7</v>
       </c>
-      <c r="AI1" t="s">
-        <v>8</v>
-      </c>
-      <c r="AJ1" t="s">
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
         <v>9</v>
       </c>
-      <c r="AK1" t="s">
+      <c r="K1" t="s">
         <v>10</v>
       </c>
-      <c r="AL1" t="s">
+      <c r="L1" t="s">
         <v>39</v>
       </c>
-      <c r="AM1" t="s">
+      <c r="M1" t="s">
         <v>11</v>
       </c>
-      <c r="AN1" t="s">
+      <c r="N1" t="s">
         <v>12</v>
       </c>
-      <c r="AO1" t="s">
+      <c r="O1" t="s">
         <v>13</v>
       </c>
-      <c r="AP1" t="s">
+      <c r="P1" t="s">
         <v>14</v>
       </c>
-      <c r="AQ1" t="s">
+      <c r="Q1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="27:43" x14ac:dyDescent="0.3">
-      <c r="AA2">
-        <v>1002000</v>
-      </c>
-      <c r="AB2">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>1002000</v>
+      </c>
+      <c r="B2">
         <v>44444</v>
       </c>
-      <c r="AC2" t="s">
+      <c r="C2" t="s">
         <v>16</v>
       </c>
-      <c r="AD2">
-        <v>8</v>
-      </c>
-      <c r="AE2">
+      <c r="D2">
+        <v>8</v>
+      </c>
+      <c r="E2">
         <v>2024</v>
       </c>
-      <c r="AF2">
+      <c r="F2">
         <v>5468</v>
       </c>
-      <c r="AG2">
-        <v>30</v>
-      </c>
-      <c r="AH2">
+      <c r="G2">
+        <v>30</v>
+      </c>
+      <c r="H2">
         <v>31</v>
       </c>
-      <c r="AI2">
+      <c r="I2">
         <v>1</v>
       </c>
-      <c r="AJ2">
-        <v>0</v>
-      </c>
-      <c r="AK2">
+      <c r="J2">
+        <v>0</v>
+      </c>
+      <c r="K2">
         <v>610001</v>
       </c>
-      <c r="AL2" t="s">
+      <c r="L2" t="s">
         <v>17</v>
       </c>
-      <c r="AM2">
+      <c r="M2">
         <v>39</v>
       </c>
-      <c r="AO2" t="s">
+      <c r="O2" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="27:43" x14ac:dyDescent="0.3">
-      <c r="AA3">
-        <v>1002000</v>
-      </c>
-      <c r="AB3">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>1002000</v>
+      </c>
+      <c r="B3">
         <v>44444</v>
       </c>
-      <c r="AC3" t="s">
+      <c r="C3" t="s">
         <v>16</v>
       </c>
-      <c r="AD3">
-        <v>8</v>
-      </c>
-      <c r="AE3">
+      <c r="D3">
+        <v>8</v>
+      </c>
+      <c r="E3">
         <v>2024</v>
       </c>
-      <c r="AF3">
+      <c r="F3">
         <v>5468</v>
       </c>
-      <c r="AG3">
-        <v>30</v>
-      </c>
-      <c r="AH3">
+      <c r="G3">
+        <v>30</v>
+      </c>
+      <c r="H3">
         <v>31</v>
       </c>
-      <c r="AI3">
+      <c r="I3">
         <v>1</v>
       </c>
-      <c r="AJ3">
-        <v>0</v>
-      </c>
-      <c r="AK3">
+      <c r="J3">
+        <v>0</v>
+      </c>
+      <c r="K3">
         <v>702901</v>
       </c>
-      <c r="AL3" t="s">
+      <c r="L3" t="s">
         <v>19</v>
       </c>
-      <c r="AM3">
+      <c r="M3">
         <v>2</v>
       </c>
-      <c r="AN3">
-        <v>0</v>
-      </c>
-      <c r="AO3" t="s">
+      <c r="N3">
+        <v>0</v>
+      </c>
+      <c r="O3" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="27:43" x14ac:dyDescent="0.3">
-      <c r="AA4">
-        <v>1002000</v>
-      </c>
-      <c r="AB4">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>1002000</v>
+      </c>
+      <c r="B4">
         <v>44444</v>
       </c>
-      <c r="AC4" t="s">
+      <c r="C4" t="s">
         <v>16</v>
       </c>
-      <c r="AD4">
-        <v>8</v>
-      </c>
-      <c r="AE4">
+      <c r="D4">
+        <v>8</v>
+      </c>
+      <c r="E4">
         <v>2024</v>
       </c>
-      <c r="AF4">
+      <c r="F4">
         <v>5468</v>
       </c>
-      <c r="AG4">
-        <v>30</v>
-      </c>
-      <c r="AH4">
+      <c r="G4">
+        <v>30</v>
+      </c>
+      <c r="H4">
         <v>31</v>
       </c>
-      <c r="AI4">
+      <c r="I4">
         <v>1</v>
       </c>
-      <c r="AJ4">
-        <v>0</v>
-      </c>
-      <c r="AK4">
+      <c r="J4">
+        <v>0</v>
+      </c>
+      <c r="K4">
         <v>702901</v>
       </c>
-      <c r="AL4" t="s">
+      <c r="L4" t="s">
         <v>19</v>
       </c>
-      <c r="AM4" t="s">
+      <c r="M4" t="s">
         <v>20</v>
       </c>
-      <c r="AN4">
-        <v>0</v>
-      </c>
-      <c r="AO4" t="s">
+      <c r="N4">
+        <v>0</v>
+      </c>
+      <c r="O4" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="27:43" x14ac:dyDescent="0.3">
-      <c r="AA5">
-        <v>1002000</v>
-      </c>
-      <c r="AB5">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>1002000</v>
+      </c>
+      <c r="B5">
         <v>44444</v>
       </c>
-      <c r="AC5" t="s">
+      <c r="C5" t="s">
         <v>16</v>
       </c>
-      <c r="AD5">
-        <v>8</v>
-      </c>
-      <c r="AE5">
+      <c r="D5">
+        <v>8</v>
+      </c>
+      <c r="E5">
         <v>2024</v>
       </c>
-      <c r="AF5">
+      <c r="F5">
         <v>5468</v>
       </c>
-      <c r="AG5">
-        <v>30</v>
-      </c>
-      <c r="AH5">
+      <c r="G5">
+        <v>30</v>
+      </c>
+      <c r="H5">
         <v>31</v>
       </c>
-      <c r="AI5">
+      <c r="I5">
         <v>1</v>
       </c>
-      <c r="AJ5">
-        <v>0</v>
-      </c>
-      <c r="AK5">
+      <c r="J5">
+        <v>0</v>
+      </c>
+      <c r="K5">
         <v>703025</v>
       </c>
-      <c r="AL5" t="s">
+      <c r="L5" t="s">
         <v>21</v>
       </c>
-      <c r="AQ5" t="s">
+      <c r="Q5" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="6" spans="27:43" x14ac:dyDescent="0.3">
-      <c r="AA6">
-        <v>1002000</v>
-      </c>
-      <c r="AB6">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>1002000</v>
+      </c>
+      <c r="B6">
         <v>44444</v>
       </c>
-      <c r="AC6" t="s">
+      <c r="C6" t="s">
         <v>16</v>
       </c>
-      <c r="AD6">
-        <v>8</v>
-      </c>
-      <c r="AE6">
+      <c r="D6">
+        <v>8</v>
+      </c>
+      <c r="E6">
         <v>2024</v>
       </c>
-      <c r="AF6">
+      <c r="F6">
         <v>5468</v>
       </c>
-      <c r="AG6">
-        <v>30</v>
-      </c>
-      <c r="AH6">
+      <c r="G6">
+        <v>30</v>
+      </c>
+      <c r="H6">
         <v>31</v>
       </c>
-      <c r="AI6">
+      <c r="I6">
         <v>1</v>
       </c>
-      <c r="AJ6">
-        <v>0</v>
-      </c>
-      <c r="AK6">
+      <c r="J6">
+        <v>0</v>
+      </c>
+      <c r="K6">
         <v>751510</v>
       </c>
-      <c r="AL6" t="s">
+      <c r="L6" t="s">
         <v>23</v>
       </c>
-      <c r="AQ6">
+      <c r="Q6">
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="27:43" x14ac:dyDescent="0.3">
-      <c r="AA7">
-        <v>1002000</v>
-      </c>
-      <c r="AB7">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>1002000</v>
+      </c>
+      <c r="B7">
         <v>44444</v>
       </c>
-      <c r="AC7" t="s">
+      <c r="C7" t="s">
         <v>16</v>
       </c>
-      <c r="AD7">
-        <v>8</v>
-      </c>
-      <c r="AE7">
+      <c r="D7">
+        <v>8</v>
+      </c>
+      <c r="E7">
         <v>2024</v>
       </c>
-      <c r="AF7">
+      <c r="F7">
         <v>5468</v>
       </c>
-      <c r="AG7">
-        <v>30</v>
-      </c>
-      <c r="AH7">
+      <c r="G7">
+        <v>30</v>
+      </c>
+      <c r="H7">
         <v>31</v>
       </c>
-      <c r="AI7">
+      <c r="I7">
         <v>1</v>
       </c>
-      <c r="AJ7">
-        <v>0</v>
-      </c>
-      <c r="AK7">
+      <c r="J7">
+        <v>0</v>
+      </c>
+      <c r="K7">
         <v>789001</v>
       </c>
-      <c r="AL7" t="s">
+      <c r="L7" t="s">
         <v>24</v>
       </c>
-      <c r="AP7">
+      <c r="P7">
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="27:43" x14ac:dyDescent="0.3">
-      <c r="AA8">
-        <v>1002000</v>
-      </c>
-      <c r="AB8">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>1002000</v>
+      </c>
+      <c r="B8">
         <v>44444</v>
       </c>
-      <c r="AC8" t="s">
+      <c r="C8" t="s">
         <v>16</v>
       </c>
-      <c r="AD8">
-        <v>8</v>
-      </c>
-      <c r="AE8">
+      <c r="D8">
+        <v>8</v>
+      </c>
+      <c r="E8">
         <v>2024</v>
       </c>
-      <c r="AF8">
+      <c r="F8">
         <v>5468</v>
       </c>
-      <c r="AG8">
-        <v>30</v>
-      </c>
-      <c r="AH8">
+      <c r="G8">
+        <v>30</v>
+      </c>
+      <c r="H8">
         <v>31</v>
       </c>
-      <c r="AI8">
+      <c r="I8">
         <v>1</v>
       </c>
-      <c r="AJ8">
-        <v>0</v>
-      </c>
-      <c r="AK8" t="s">
+      <c r="J8">
+        <v>0</v>
+      </c>
+      <c r="K8" t="s">
         <v>25</v>
       </c>
-      <c r="AL8" t="s">
+      <c r="L8" t="s">
         <v>26</v>
       </c>
-      <c r="AP8">
+      <c r="P8">
         <v>9000</v>
       </c>
     </row>
-    <row r="9" spans="27:43" x14ac:dyDescent="0.3">
-      <c r="AA9">
-        <v>1002000</v>
-      </c>
-      <c r="AB9">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>1002000</v>
+      </c>
+      <c r="B9">
         <v>44444</v>
       </c>
-      <c r="AC9" t="s">
+      <c r="C9" t="s">
         <v>16</v>
       </c>
-      <c r="AD9">
-        <v>8</v>
-      </c>
-      <c r="AE9">
+      <c r="D9">
+        <v>8</v>
+      </c>
+      <c r="E9">
         <v>2024</v>
       </c>
-      <c r="AF9">
+      <c r="F9">
         <v>5468</v>
       </c>
-      <c r="AG9">
-        <v>30</v>
-      </c>
-      <c r="AH9">
+      <c r="G9">
+        <v>30</v>
+      </c>
+      <c r="H9">
         <v>31</v>
       </c>
-      <c r="AI9">
+      <c r="I9">
         <v>1</v>
       </c>
-      <c r="AJ9">
-        <v>0</v>
-      </c>
-      <c r="AK9" t="s">
+      <c r="J9">
+        <v>0</v>
+      </c>
+      <c r="K9" t="s">
         <v>27</v>
       </c>
-      <c r="AL9" t="s">
+      <c r="L9" t="s">
         <v>28</v>
       </c>
-      <c r="AQ9">
+      <c r="Q9">
         <v>9000</v>
       </c>
     </row>
-    <row r="10" spans="27:43" x14ac:dyDescent="0.3">
-      <c r="AA10">
-        <v>1002000</v>
-      </c>
-      <c r="AB10">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>1002000</v>
+      </c>
+      <c r="B10">
         <v>44444</v>
       </c>
-      <c r="AC10" t="s">
+      <c r="C10" t="s">
         <v>16</v>
       </c>
-      <c r="AD10">
-        <v>8</v>
-      </c>
-      <c r="AE10">
+      <c r="D10">
+        <v>8</v>
+      </c>
+      <c r="E10">
         <v>2024</v>
       </c>
-      <c r="AF10">
+      <c r="F10">
         <v>5468</v>
       </c>
-      <c r="AG10">
-        <v>30</v>
-      </c>
-      <c r="AH10">
+      <c r="G10">
+        <v>30</v>
+      </c>
+      <c r="H10">
         <v>31</v>
       </c>
-      <c r="AI10">
+      <c r="I10">
         <v>1</v>
       </c>
-      <c r="AJ10">
-        <v>0</v>
-      </c>
-      <c r="AK10" t="s">
+      <c r="J10">
+        <v>0</v>
+      </c>
+      <c r="K10" t="s">
         <v>29</v>
       </c>
-      <c r="AL10" t="s">
-        <v>30</v>
-      </c>
-      <c r="AP10">
+      <c r="L10" t="s">
+        <v>30</v>
+      </c>
+      <c r="P10">
         <v>9000</v>
       </c>
     </row>
-    <row r="11" spans="27:43" x14ac:dyDescent="0.3">
-      <c r="AA11">
-        <v>1002000</v>
-      </c>
-      <c r="AB11">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>1002000</v>
+      </c>
+      <c r="B11">
         <v>44444</v>
       </c>
-      <c r="AC11" t="s">
+      <c r="C11" t="s">
         <v>16</v>
       </c>
-      <c r="AD11">
-        <v>8</v>
-      </c>
-      <c r="AE11">
+      <c r="D11">
+        <v>8</v>
+      </c>
+      <c r="E11">
         <v>2024</v>
       </c>
-      <c r="AF11">
+      <c r="F11">
         <v>5468</v>
       </c>
-      <c r="AG11">
-        <v>30</v>
-      </c>
-      <c r="AH11">
+      <c r="G11">
+        <v>30</v>
+      </c>
+      <c r="H11">
         <v>31</v>
       </c>
-      <c r="AI11">
+      <c r="I11">
         <v>1</v>
       </c>
-      <c r="AJ11">
-        <v>0</v>
-      </c>
-      <c r="AK11" t="s">
+      <c r="J11">
+        <v>0</v>
+      </c>
+      <c r="K11" t="s">
         <v>31</v>
       </c>
-      <c r="AL11" t="s">
+      <c r="L11" t="s">
         <v>32</v>
       </c>
-      <c r="AQ11">
+      <c r="Q11">
         <v>9000</v>
       </c>
     </row>
-    <row r="12" spans="27:43" x14ac:dyDescent="0.3">
-      <c r="AA12">
-        <v>1002000</v>
-      </c>
-      <c r="AB12">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>1002000</v>
+      </c>
+      <c r="B12">
         <v>44444</v>
       </c>
-      <c r="AC12" t="s">
+      <c r="C12" t="s">
         <v>16</v>
       </c>
-      <c r="AD12">
-        <v>8</v>
-      </c>
-      <c r="AE12">
+      <c r="D12">
+        <v>8</v>
+      </c>
+      <c r="E12">
         <v>2024</v>
       </c>
-      <c r="AF12">
+      <c r="F12">
         <v>5468</v>
       </c>
-      <c r="AG12">
-        <v>30</v>
-      </c>
-      <c r="AH12">
+      <c r="G12">
+        <v>30</v>
+      </c>
+      <c r="H12">
         <v>31</v>
       </c>
-      <c r="AI12">
+      <c r="I12">
         <v>1</v>
       </c>
-      <c r="AJ12">
-        <v>0</v>
-      </c>
-      <c r="AK12" t="s">
+      <c r="J12">
+        <v>0</v>
+      </c>
+      <c r="K12" t="s">
         <v>33</v>
       </c>
-      <c r="AL12" t="s">
+      <c r="L12" t="s">
         <v>34</v>
       </c>
-      <c r="AP12">
+      <c r="P12">
         <v>9000</v>
       </c>
     </row>
-    <row r="13" spans="27:43" x14ac:dyDescent="0.3">
-      <c r="AA13">
-        <v>1002000</v>
-      </c>
-      <c r="AB13">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>1002000</v>
+      </c>
+      <c r="B13">
         <v>44444</v>
       </c>
-      <c r="AC13" t="s">
+      <c r="C13" t="s">
         <v>16</v>
       </c>
-      <c r="AD13">
-        <v>8</v>
-      </c>
-      <c r="AE13">
+      <c r="D13">
+        <v>8</v>
+      </c>
+      <c r="E13">
         <v>2024</v>
       </c>
-      <c r="AF13">
+      <c r="F13">
         <v>5468</v>
       </c>
-      <c r="AG13">
-        <v>30</v>
-      </c>
-      <c r="AH13">
+      <c r="G13">
+        <v>30</v>
+      </c>
+      <c r="H13">
         <v>31</v>
       </c>
-      <c r="AI13">
+      <c r="I13">
         <v>1</v>
       </c>
-      <c r="AJ13">
-        <v>0</v>
-      </c>
-      <c r="AK13" t="s">
+      <c r="J13">
+        <v>0</v>
+      </c>
+      <c r="K13" t="s">
         <v>35</v>
       </c>
-      <c r="AL13" t="s">
+      <c r="L13" t="s">
         <v>36</v>
       </c>
-      <c r="AM13">
+      <c r="M13">
         <v>25</v>
       </c>
     </row>
-    <row r="14" spans="27:43" x14ac:dyDescent="0.3">
-      <c r="AA14">
-        <v>1002000</v>
-      </c>
-      <c r="AB14">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>1002000</v>
+      </c>
+      <c r="B14">
         <v>555555</v>
       </c>
-      <c r="AC14" t="s">
+      <c r="C14" t="s">
         <v>37</v>
       </c>
-      <c r="AD14">
-        <v>8</v>
-      </c>
-      <c r="AL14" t="s">
+      <c r="D14">
+        <v>8</v>
+      </c>
+      <c r="L14" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="15" spans="27:43" x14ac:dyDescent="0.3">
-      <c r="AA15">
-        <v>1002000</v>
-      </c>
-      <c r="AB15">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>1002000</v>
+      </c>
+      <c r="B15">
         <v>555555</v>
       </c>
-      <c r="AC15" t="s">
+      <c r="C15" t="s">
         <v>37</v>
       </c>
-      <c r="AD15">
+      <c r="D15">
         <v>9</v>
       </c>
-      <c r="AL15" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="16" spans="27:43" x14ac:dyDescent="0.3">
-      <c r="AA16">
-        <v>1002000</v>
-      </c>
-      <c r="AB16">
+      <c r="L15" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>1002000</v>
+      </c>
+      <c r="B16">
         <v>6666</v>
       </c>
-      <c r="AC16" t="s">
+      <c r="C16" t="s">
         <v>38</v>
       </c>
-      <c r="AD16">
+      <c r="D16">
         <v>9</v>
       </c>
-      <c r="AL16" t="s">
+      <c r="L16" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="17" spans="27:38" x14ac:dyDescent="0.3">
-      <c r="AA17">
-        <v>1002000</v>
-      </c>
-      <c r="AB17">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <v>1002000</v>
+      </c>
+      <c r="B17">
         <v>6666</v>
       </c>
-      <c r="AC17" t="s">
+      <c r="C17" t="s">
         <v>38</v>
       </c>
-      <c r="AD17">
+      <c r="D17">
         <v>9</v>
       </c>
-      <c r="AL17" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="18" spans="27:38" x14ac:dyDescent="0.3">
-      <c r="AA18">
-        <v>1002000</v>
-      </c>
-      <c r="AB18">
+      <c r="L17" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <v>1002000</v>
+      </c>
+      <c r="B18">
         <v>6666</v>
       </c>
-      <c r="AC18" t="s">
+      <c r="C18" t="s">
         <v>38</v>
       </c>
-      <c r="AD18">
-        <v>8</v>
-      </c>
-      <c r="AL18" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="19" spans="27:38" x14ac:dyDescent="0.3">
-      <c r="AA19">
-        <v>1002000</v>
-      </c>
-      <c r="AB19">
+      <c r="D18">
+        <v>8</v>
+      </c>
+      <c r="L18" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A19">
+        <v>1002000</v>
+      </c>
+      <c r="B19">
         <v>6666</v>
       </c>
-      <c r="AC19" t="s">
+      <c r="C19" t="s">
         <v>38</v>
       </c>
-      <c r="AD19">
-        <v>8</v>
-      </c>
-      <c r="AL19" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="20" spans="27:38" x14ac:dyDescent="0.3">
-      <c r="AA20">
-        <v>1002000</v>
-      </c>
-      <c r="AB20">
+      <c r="D19">
+        <v>8</v>
+      </c>
+      <c r="L19" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A20">
+        <v>1002000</v>
+      </c>
+      <c r="B20">
         <v>777</v>
       </c>
-      <c r="AC20" t="s">
+      <c r="C20" t="s">
         <v>40</v>
       </c>
-      <c r="AD20">
+      <c r="D20">
         <v>4</v>
       </c>
-      <c r="AL20" t="s">
+      <c r="L20" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="21" spans="27:38" x14ac:dyDescent="0.3">
-      <c r="AA21">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A21">
         <v>1003000</v>
       </c>
-      <c r="AB21">
+      <c r="B21">
         <v>777</v>
       </c>
-      <c r="AC21" t="s">
+      <c r="C21" t="s">
         <v>40</v>
       </c>
-      <c r="AD21">
+      <c r="D21">
         <v>3</v>
       </c>
-      <c r="AL21" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="22" spans="27:38" x14ac:dyDescent="0.3">
-      <c r="AA22">
+      <c r="L21" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A22">
         <v>1003000</v>
       </c>
-      <c r="AB22">
+      <c r="B22">
         <v>777</v>
       </c>
-      <c r="AC22" t="s">
+      <c r="C22" t="s">
         <v>40</v>
       </c>
-      <c r="AD22">
+      <c r="D22">
         <v>3</v>
       </c>
-      <c r="AL22" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="23" spans="27:38" x14ac:dyDescent="0.3">
-      <c r="AA23">
+      <c r="L22" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A23">
         <v>1003000</v>
       </c>
-      <c r="AB23">
+      <c r="B23">
         <v>222</v>
       </c>
-      <c r="AC23" t="s">
+      <c r="C23" t="s">
         <v>41</v>
       </c>
-      <c r="AD23">
+      <c r="D23">
         <v>9</v>
       </c>
-      <c r="AL23" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="24" spans="27:38" x14ac:dyDescent="0.3">
-      <c r="AA24">
+      <c r="L23" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A24">
         <v>1003000</v>
       </c>
-      <c r="AB24">
+      <c r="B24">
         <v>222</v>
       </c>
-      <c r="AC24" t="s">
+      <c r="C24" t="s">
         <v>41</v>
       </c>
-      <c r="AD24">
+      <c r="D24">
         <v>4</v>
       </c>
-      <c r="AL24" t="s">
+      <c r="L24" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="25" spans="27:38" x14ac:dyDescent="0.3">
-      <c r="AA25">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A25">
         <v>1003000</v>
       </c>
-      <c r="AB25">
+      <c r="B25">
         <v>33</v>
       </c>
-      <c r="AC25" t="s">
+      <c r="C25" t="s">
         <v>42</v>
       </c>
-      <c r="AD25">
+      <c r="D25">
         <v>6</v>
       </c>
-      <c r="AL25" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="26" spans="27:38" x14ac:dyDescent="0.3">
-      <c r="AA26">
+      <c r="L25" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A26">
         <v>1003000</v>
       </c>
-      <c r="AB26">
+      <c r="B26">
         <v>33</v>
       </c>
-      <c r="AC26" t="s">
+      <c r="C26" t="s">
         <v>42</v>
       </c>
-      <c r="AD26">
+      <c r="D26">
         <v>6</v>
       </c>
-      <c r="AL26" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="27" spans="27:38" x14ac:dyDescent="0.3">
-      <c r="AA27">
+      <c r="L26" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A27">
         <v>1003000</v>
       </c>
-      <c r="AB27">
+      <c r="B27">
         <v>18</v>
       </c>
-      <c r="AC27" t="s">
+      <c r="C27" t="s">
         <v>43</v>
       </c>
-      <c r="AD27">
-        <v>8</v>
-      </c>
-      <c r="AL27" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="28" spans="27:38" x14ac:dyDescent="0.3">
-      <c r="AA28">
+      <c r="D27">
+        <v>8</v>
+      </c>
+      <c r="L27" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A28">
         <v>1003000</v>
       </c>
-      <c r="AB28">
+      <c r="B28">
         <v>18</v>
       </c>
-      <c r="AC28" t="s">
+      <c r="C28" t="s">
         <v>43</v>
       </c>
-      <c r="AD28">
-        <v>8</v>
-      </c>
-      <c r="AL28" t="s">
+      <c r="D28">
+        <v>8</v>
+      </c>
+      <c r="L28" t="s">
         <v>30</v>
       </c>
     </row>

</xml_diff>